<commit_message>
I had mislabled this so the man and max were switched around and I needed to fix them
</commit_message>
<xml_diff>
--- a/data/Peromyscus_FMNH_FW.xlsx
+++ b/data/Peromyscus_FMNH_FW.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://oregonstateuniversity-my.sharepoint.com/personal/morrisph_oregonstate_edu/Documents/Projects/Peromyscus Measurements/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://oregonstateuniversity-my.sharepoint.com/personal/morrisph_oregonstate_edu/Documents/Analytical Workflows/AnalyticalWorkflowsProject-Morris/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="8_{6CAB63B6-6E5F-49C4-9FD4-A2EFC33158A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93628000-7C35-484C-82E7-E459C75EE0D9}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="8_{6CAB63B6-6E5F-49C4-9FD4-A2EFC33158A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC14F7DA-AAC2-4EBD-96DD-567A84CB5FF1}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{D4FA0AB5-0EFE-4A7F-9470-C6FFDD65D3DF}"/>
   </bookViews>
@@ -250,7 +250,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,12 +264,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -745,7 +739,7 @@
   <dimension ref="A1:P114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,37 +760,37 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="N1" s="4" t="s">
         <v>3</v>

</xml_diff>